<commit_message>
update profils, add mapping et exemples 0b5190d6eea292b984f419dc701e01471132ef76
</commit_message>
<xml_diff>
--- a/389-mapping---projet-personnalisé/ig/StructureDefinition-tddui-careplan-reference.xlsx
+++ b/389-mapping---projet-personnalisé/ig/StructureDefinition-tddui-careplan-reference.xlsx
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Lien vers le projet personnel</t>
+    <t>Lien vers le projet personnalisé</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-18T14:30:08+00:00</t>
+    <t>2025-11-18T15:24:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Liens vers le projet personnel, utilisables dans le profil TDDUIGoalObjectif.</t>
+    <t>Liens vers le projet personnalisé, utilisables dans le profil TDDUIGoalObjectif.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>

<commit_message>
update identifier value & system 50666c4037d2e9c165f5bfe840d0452092a65d7c
</commit_message>
<xml_diff>
--- a/389-mapping---projet-personnalisé/ig/StructureDefinition-tddui-careplan-reference.xlsx
+++ b/389-mapping---projet-personnalisé/ig/StructureDefinition-tddui-careplan-reference.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-20T16:06:37+00:00</t>
+    <t>2025-11-21T09:00:00+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -331,7 +331,7 @@
     <t>Extension.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-careplan-projet-personalise)
+    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-careplan-projet-personnalise)
 </t>
   </si>
   <si>
@@ -674,7 +674,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="85.2421875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="86.23828125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>